<commit_message>
inventory recalculation when canceling expense seems to be ok, but buggy when re-adding the expense.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/material_expense_cancelation_log_test_case_22_state_3_mm6.xlsx
+++ b/soberano/test_cases/material_expense_cancelation_log_test_case_22_state_3_mm6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mw10" sheetId="1" state="visible" r:id="rId2"/>
@@ -238,11 +238,11 @@
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J26" activeCellId="1" sqref="J13 J26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J20" activeCellId="1" sqref="J15 J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.45"/>
@@ -1403,11 +1403,11 @@
   </sheetPr>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M14" activeCellId="1" sqref="J13 M14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H14" activeCellId="1" sqref="J15 H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.08"/>
@@ -1692,11 +1692,11 @@
   </sheetPr>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="1" sqref="J13 B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J5" activeCellId="1" sqref="J15 J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.08"/>
@@ -1704,7 +1704,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.11"/>
   </cols>
@@ -2024,10 +2024,10 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="1" sqref="J13 L9"/>
+      <selection pane="topLeft" activeCell="L13" activeCellId="1" sqref="J15 L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.22"/>

</xml_diff>